<commit_message>
- Exposed to the top LTPI modules data channel and CSR access signals - Increased data channel timeout to 10ms - Synchronize lvds phy reset signals - Changed SMBUSs timing parameters - Added gpio ltpi top module and ltpi top module parameterized unit test - Updated documentation files
Signed-off-by :Katarzyna Krzewska <katarzyna.krzewska@intel.com>
</commit_message>
<xml_diff>
--- a/docs/LTPI_test_plan.xlsx
+++ b/docs/LTPI_test_plan.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/katarzyna_krzewska_intel_com/Documents/Documents/LTPI/LTPI_dokumentacja/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/katarzyna_krzewska_intel_com/Documents/Documents/LTPI/LTPI_dokumentacja/LTPI_src_OCP_release/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="528" documentId="8_{1719A915-AC1B-49BB-AA9D-1482FFA7DE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{174E16DD-1604-45CD-AAB5-4C53B72D13CE}"/>
+  <xr:revisionPtr revIDLastSave="615" documentId="8_{1719A915-AC1B-49BB-AA9D-1482FFA7DE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A543862-F5AF-4F6F-8638-5DC670249272}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B27309D5-33D0-42FB-BA45-6062C8749EE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{B27309D5-33D0-42FB-BA45-6062C8749EE3}"/>
   </bookViews>
   <sheets>
     <sheet name="LTPI 1.0" sheetId="1" r:id="rId1"/>
+    <sheet name="LTPI 1.09" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="172">
   <si>
     <t>Test nb</t>
   </si>
@@ -538,13 +539,25 @@
   </si>
   <si>
     <t>mgmt_data_channel_direct_mm_unit_test.sv</t>
+  </si>
+  <si>
+    <t>LTPI_top_gpio_unit_test.sv</t>
+  </si>
+  <si>
+    <t>Set normal and low latancy GPIO</t>
+  </si>
+  <si>
+    <t>ltpi_top_param_unit_test.sv</t>
+  </si>
+  <si>
+    <t>This test is only valid with "LTPI top controller BMC proposal connection" Tabel 2 User guide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -604,8 +617,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -640,8 +660,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -823,13 +849,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -851,9 +927,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -871,7 +946,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -914,7 +989,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -927,6 +1001,67 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -947,9 +1082,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -987,7 +1122,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1093,7 +1228,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1235,7 +1370,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1245,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFFD11D-961A-4DE5-92A2-AC8834FBB74E}">
   <dimension ref="A1:F150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B153" sqref="B153"/>
+    <sheetView topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B153" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,27 +1396,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1292,10 +1427,10 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="21"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="21">
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -1306,10 +1441,10 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="21"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
+      <c r="A4" s="19">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1320,10 +1455,10 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="23"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -1334,10 +1469,10 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="23"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="A6" s="19">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1348,10 +1483,10 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="21"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="21">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -1362,10 +1497,10 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="21"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
+      <c r="A8" s="19">
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1376,10 +1511,10 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="21"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="21">
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -1390,10 +1525,10 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="21"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="20">
+      <c r="A10" s="19">
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1404,10 +1539,10 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="21"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="21">
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -1418,10 +1553,10 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="21"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="20">
+      <c r="A12" s="19">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -1432,10 +1567,10 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="21"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
+      <c r="A13" s="21">
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -1446,10 +1581,10 @@
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="21"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+      <c r="A14" s="19">
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1460,10 +1595,10 @@
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="23"/>
+      <c r="F14" s="22"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+      <c r="A15" s="21">
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -1474,10 +1609,10 @@
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="23"/>
+      <c r="F15" s="22"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
+      <c r="A16" s="19">
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1488,10 +1623,10 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="23"/>
+      <c r="F16" s="22"/>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
+      <c r="A17" s="21">
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -1502,12 +1637,12 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="22" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
+      <c r="A18" s="19">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -1518,10 +1653,10 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="23"/>
+      <c r="F18" s="22"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
+      <c r="A19" s="21">
         <v>18</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -1532,10 +1667,10 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="21"/>
+      <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
+      <c r="A20" s="19">
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1546,10 +1681,10 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="23"/>
+      <c r="F20" s="22"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
+      <c r="A21" s="21">
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -1560,10 +1695,10 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="21"/>
+      <c r="F21" s="20"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
+      <c r="A22" s="19">
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -1574,10 +1709,10 @@
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="23"/>
+      <c r="F22" s="22"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
+      <c r="A23" s="21">
         <v>22</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -1588,10 +1723,10 @@
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="21"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20">
+      <c r="A24" s="19">
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -1602,12 +1737,12 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="23" t="s">
+      <c r="F24" s="22" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
+      <c r="A25" s="21">
         <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -1618,10 +1753,10 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="23"/>
+      <c r="F25" s="22"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="20">
+      <c r="A26" s="19">
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -1632,10 +1767,10 @@
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="21"/>
+      <c r="F26" s="20"/>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="22">
+      <c r="A27" s="21">
         <v>26</v>
       </c>
       <c r="B27" s="10" t="s">
@@ -1646,33 +1781,33 @@
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="21"/>
+      <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="24">
+      <c r="A28" s="23">
         <v>27</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="28"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="27"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="13"/>
+      <c r="B30" s="7"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1680,63 +1815,63 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
-      <c r="B31" s="29"/>
+      <c r="B31" s="28"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="32" t="s">
+      <c r="E32" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="33" t="s">
+      <c r="F32" s="32" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="39">
+      <c r="A33" s="38">
         <v>1</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="39" t="s">
         <v>165</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="34"/>
+      <c r="F33" s="33"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="37">
+      <c r="A34" s="36">
         <f>A33+1</f>
         <v>2</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="37" t="s">
         <v>8</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="23"/>
+      <c r="F34" s="22"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="37">
+      <c r="A35" s="36">
         <f t="shared" ref="A35:A64" si="0">A34+1</f>
         <v>3</v>
       </c>
@@ -1748,10 +1883,10 @@
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="23"/>
+      <c r="F35" s="22"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="37">
+      <c r="A36" s="36">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1763,10 +1898,10 @@
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="23"/>
+      <c r="F36" s="22"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="37">
+      <c r="A37" s="36">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1778,160 +1913,160 @@
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="23"/>
+      <c r="F37" s="22"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="39">
+      <c r="A38" s="38">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="41" t="s">
+      <c r="C38" s="40" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="23"/>
+      <c r="F38" s="22"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="39">
+      <c r="A39" s="38">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B39" s="41" t="s">
+      <c r="B39" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="40" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="23"/>
+      <c r="F39" s="22"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="39">
+      <c r="A40" s="38">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B40" s="41" t="s">
+      <c r="B40" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C40" s="40" t="s">
         <v>15</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="23"/>
+      <c r="F40" s="22"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="39">
+      <c r="A41" s="38">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="41" t="s">
+      <c r="C41" s="40" t="s">
         <v>16</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="23"/>
+      <c r="F41" s="22"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="39">
+      <c r="A42" s="38">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="40" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="23"/>
+      <c r="F42" s="22"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="39">
+      <c r="A43" s="38">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="41" t="s">
+      <c r="C43" s="40" t="s">
         <v>18</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="23"/>
+      <c r="F43" s="22"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="39">
+      <c r="A44" s="38">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="40" t="s">
         <v>19</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="23"/>
+      <c r="F44" s="22"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="39">
+      <c r="A45" s="38">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="41" t="s">
+      <c r="C45" s="40" t="s">
         <v>20</v>
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="23"/>
+      <c r="F45" s="22"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="39">
+      <c r="A46" s="38">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B46" s="41" t="s">
+      <c r="B46" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="41" t="s">
+      <c r="C46" s="40" t="s">
         <v>21</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="23"/>
+      <c r="F46" s="22"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="39">
+      <c r="A47" s="38">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="41" t="s">
+      <c r="C47" s="40" t="s">
         <v>22</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="23"/>
+      <c r="F47" s="22"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="37">
+      <c r="A48" s="36">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -1943,55 +2078,55 @@
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="23"/>
+      <c r="F48" s="22"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="39">
+      <c r="A49" s="38">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B49" s="41" t="s">
+      <c r="B49" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C49" s="41" t="s">
+      <c r="C49" s="40" t="s">
         <v>25</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="23"/>
+      <c r="F49" s="22"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="39">
+      <c r="A50" s="38">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="41" t="s">
+      <c r="C50" s="40" t="s">
         <v>26</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="23"/>
+      <c r="F50" s="22"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="39">
+      <c r="A51" s="38">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B51" s="41" t="s">
+      <c r="B51" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C51" s="41" t="s">
+      <c r="C51" s="40" t="s">
         <v>27</v>
       </c>
       <c r="D51" s="8"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="23"/>
+      <c r="F51" s="22"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="37">
+      <c r="A52" s="36">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -2003,10 +2138,10 @@
       </c>
       <c r="D52" s="8"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="23"/>
+      <c r="F52" s="22"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="37">
+      <c r="A53" s="36">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -2018,10 +2153,10 @@
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="23"/>
+      <c r="F53" s="22"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="37">
+      <c r="A54" s="36">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
@@ -2033,10 +2168,10 @@
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="23"/>
+      <c r="F54" s="22"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="37">
+      <c r="A55" s="36">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -2048,70 +2183,70 @@
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="3"/>
-      <c r="F55" s="23"/>
+      <c r="F55" s="22"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="39">
+      <c r="A56" s="38">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B56" s="41" t="s">
+      <c r="B56" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="41" t="s">
+      <c r="C56" s="40" t="s">
         <v>34</v>
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="23"/>
+      <c r="F56" s="22"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="39">
+      <c r="A57" s="38">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C57" s="41" t="s">
+      <c r="C57" s="40" t="s">
         <v>35</v>
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="23"/>
+      <c r="F57" s="22"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="39">
+      <c r="A58" s="38">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B58" s="41" t="s">
+      <c r="B58" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C58" s="41" t="s">
+      <c r="C58" s="40" t="s">
         <v>121</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="23"/>
+      <c r="F58" s="22"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="39">
+      <c r="A59" s="38">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C59" s="41" t="s">
+      <c r="C59" s="40" t="s">
         <v>120</v>
       </c>
       <c r="D59" s="8"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="23"/>
+      <c r="F59" s="22"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="37">
+      <c r="A60" s="36">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -2123,10 +2258,10 @@
       </c>
       <c r="D60" s="8"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="23"/>
+      <c r="F60" s="22"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="37">
+      <c r="A61" s="36">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
@@ -2138,10 +2273,10 @@
       </c>
       <c r="D61" s="8"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="23"/>
+      <c r="F61" s="22"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="37">
+      <c r="A62" s="36">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -2153,10 +2288,10 @@
       </c>
       <c r="D62" s="8"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="23"/>
+      <c r="F62" s="22"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="37">
+      <c r="A63" s="36">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
@@ -2168,10 +2303,10 @@
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="23"/>
+      <c r="F63" s="22"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="37">
+      <c r="A64" s="36">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -2183,10 +2318,10 @@
       </c>
       <c r="D64" s="8"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="23"/>
+      <c r="F64" s="22"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="37">
+      <c r="A65" s="36">
         <f t="shared" ref="A65:A74" si="1">A64+1</f>
         <v>33</v>
       </c>
@@ -2198,10 +2333,10 @@
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="3"/>
-      <c r="F65" s="23"/>
+      <c r="F65" s="22"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="37">
+      <c r="A66" s="36">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
@@ -2213,10 +2348,10 @@
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="23"/>
+      <c r="F66" s="22"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="37">
+      <c r="A67" s="36">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
@@ -2228,10 +2363,10 @@
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="3"/>
-      <c r="F67" s="23"/>
+      <c r="F67" s="22"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="37">
+      <c r="A68" s="36">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
@@ -2243,10 +2378,10 @@
       </c>
       <c r="D68" s="8"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="23"/>
+      <c r="F68" s="22"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="37">
+      <c r="A69" s="36">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
@@ -2258,10 +2393,10 @@
       </c>
       <c r="D69" s="8"/>
       <c r="E69" s="3"/>
-      <c r="F69" s="23"/>
+      <c r="F69" s="22"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="37">
+      <c r="A70" s="36">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
@@ -2273,10 +2408,10 @@
       </c>
       <c r="D70" s="8"/>
       <c r="E70" s="3"/>
-      <c r="F70" s="23"/>
+      <c r="F70" s="22"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="37">
+      <c r="A71" s="36">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
@@ -2288,10 +2423,10 @@
       </c>
       <c r="D71" s="8"/>
       <c r="E71" s="3"/>
-      <c r="F71" s="23"/>
+      <c r="F71" s="22"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="37">
+      <c r="A72" s="36">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
@@ -2303,10 +2438,10 @@
       </c>
       <c r="D72" s="8"/>
       <c r="E72" s="3"/>
-      <c r="F72" s="23"/>
+      <c r="F72" s="22"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="37">
+      <c r="A73" s="36">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
@@ -2318,10 +2453,10 @@
       </c>
       <c r="D73" s="8"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="23"/>
+      <c r="F73" s="22"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="37">
+      <c r="A74" s="36">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
@@ -2333,10 +2468,10 @@
       </c>
       <c r="D74" s="8"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="23"/>
+      <c r="F74" s="22"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="37">
+      <c r="A75" s="36">
         <f>A74+1</f>
         <v>43</v>
       </c>
@@ -2348,10 +2483,10 @@
       </c>
       <c r="D75" s="8"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="23"/>
+      <c r="F75" s="22"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="37">
+      <c r="A76" s="36">
         <f t="shared" ref="A76:A141" si="2">A75+1</f>
         <v>44</v>
       </c>
@@ -2363,10 +2498,10 @@
       </c>
       <c r="D76" s="8"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="23"/>
+      <c r="F76" s="22"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="37">
+      <c r="A77" s="36">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
@@ -2378,10 +2513,10 @@
       </c>
       <c r="D77" s="8"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="23"/>
+      <c r="F77" s="22"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="37">
+      <c r="A78" s="36">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
@@ -2393,55 +2528,55 @@
       </c>
       <c r="D78" s="8"/>
       <c r="E78" s="3"/>
-      <c r="F78" s="23"/>
+      <c r="F78" s="22"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="39">
+      <c r="A79" s="38">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="B79" s="41" t="s">
+      <c r="B79" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C79" s="41" t="s">
+      <c r="C79" s="40" t="s">
         <v>48</v>
       </c>
       <c r="D79" s="8"/>
       <c r="E79" s="3"/>
-      <c r="F79" s="23"/>
+      <c r="F79" s="22"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="39">
+      <c r="A80" s="38">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="B80" s="41" t="s">
+      <c r="B80" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C80" s="41" t="s">
+      <c r="C80" s="40" t="s">
         <v>49</v>
       </c>
       <c r="D80" s="8"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="23"/>
+      <c r="F80" s="22"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="39">
+      <c r="A81" s="38">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="B81" s="41" t="s">
+      <c r="B81" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C81" s="41" t="s">
+      <c r="C81" s="40" t="s">
         <v>134</v>
       </c>
       <c r="D81" s="8"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="23"/>
+      <c r="F81" s="22"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="37">
+      <c r="A82" s="36">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
@@ -2453,10 +2588,10 @@
       </c>
       <c r="D82" s="8"/>
       <c r="E82" s="3"/>
-      <c r="F82" s="23"/>
+      <c r="F82" s="22"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="37">
+      <c r="A83" s="36">
         <f t="shared" si="2"/>
         <v>51</v>
       </c>
@@ -2468,10 +2603,10 @@
       </c>
       <c r="D83" s="8"/>
       <c r="E83" s="3"/>
-      <c r="F83" s="23"/>
+      <c r="F83" s="22"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="37">
+      <c r="A84" s="36">
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
@@ -2483,10 +2618,10 @@
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="3"/>
-      <c r="F84" s="23"/>
+      <c r="F84" s="22"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="37">
+      <c r="A85" s="36">
         <f t="shared" si="2"/>
         <v>53</v>
       </c>
@@ -2498,10 +2633,10 @@
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="3"/>
-      <c r="F85" s="23"/>
+      <c r="F85" s="22"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="37">
+      <c r="A86" s="36">
         <f t="shared" si="2"/>
         <v>54</v>
       </c>
@@ -2513,10 +2648,10 @@
       </c>
       <c r="D86" s="8"/>
       <c r="E86" s="3"/>
-      <c r="F86" s="23"/>
+      <c r="F86" s="22"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="37">
+      <c r="A87" s="36">
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
@@ -2528,10 +2663,10 @@
       </c>
       <c r="D87" s="8"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="23"/>
+      <c r="F87" s="22"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="37">
+      <c r="A88" s="36">
         <f t="shared" si="2"/>
         <v>56</v>
       </c>
@@ -2543,10 +2678,10 @@
       </c>
       <c r="D88" s="8"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="23"/>
+      <c r="F88" s="22"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="37">
+      <c r="A89" s="36">
         <f t="shared" si="2"/>
         <v>57</v>
       </c>
@@ -2558,10 +2693,10 @@
       </c>
       <c r="D89" s="8"/>
       <c r="E89" s="3"/>
-      <c r="F89" s="23"/>
+      <c r="F89" s="22"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="37">
+      <c r="A90" s="36">
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
@@ -2573,10 +2708,10 @@
       </c>
       <c r="D90" s="8"/>
       <c r="E90" s="3"/>
-      <c r="F90" s="23"/>
+      <c r="F90" s="22"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="37">
+      <c r="A91" s="36">
         <f t="shared" si="2"/>
         <v>59</v>
       </c>
@@ -2588,10 +2723,10 @@
       </c>
       <c r="D91" s="8"/>
       <c r="E91" s="3"/>
-      <c r="F91" s="23"/>
+      <c r="F91" s="22"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="37">
+      <c r="A92" s="36">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
@@ -2603,10 +2738,10 @@
       </c>
       <c r="D92" s="8"/>
       <c r="E92" s="3"/>
-      <c r="F92" s="23"/>
+      <c r="F92" s="22"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="37">
+      <c r="A93" s="36">
         <f t="shared" si="2"/>
         <v>61</v>
       </c>
@@ -2618,10 +2753,10 @@
       </c>
       <c r="D93" s="8"/>
       <c r="E93" s="3"/>
-      <c r="F93" s="23"/>
+      <c r="F93" s="22"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="37">
+      <c r="A94" s="36">
         <f t="shared" si="2"/>
         <v>62</v>
       </c>
@@ -2633,10 +2768,10 @@
       </c>
       <c r="D94" s="8"/>
       <c r="E94" s="3"/>
-      <c r="F94" s="23"/>
+      <c r="F94" s="22"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="37">
+      <c r="A95" s="36">
         <f t="shared" si="2"/>
         <v>63</v>
       </c>
@@ -2648,10 +2783,10 @@
       </c>
       <c r="D95" s="8"/>
       <c r="E95" s="3"/>
-      <c r="F95" s="23"/>
+      <c r="F95" s="22"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="37">
+      <c r="A96" s="36">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
@@ -2663,10 +2798,10 @@
       </c>
       <c r="D96" s="8"/>
       <c r="E96" s="3"/>
-      <c r="F96" s="23"/>
+      <c r="F96" s="22"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="37">
+      <c r="A97" s="36">
         <f t="shared" si="2"/>
         <v>65</v>
       </c>
@@ -2678,10 +2813,10 @@
       </c>
       <c r="D97" s="8"/>
       <c r="E97" s="3"/>
-      <c r="F97" s="23"/>
+      <c r="F97" s="22"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="37">
+      <c r="A98" s="36">
         <f t="shared" si="2"/>
         <v>66</v>
       </c>
@@ -2693,10 +2828,10 @@
       </c>
       <c r="D98" s="8"/>
       <c r="E98" s="3"/>
-      <c r="F98" s="23"/>
+      <c r="F98" s="22"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="37">
+      <c r="A99" s="36">
         <f t="shared" si="2"/>
         <v>67</v>
       </c>
@@ -2708,10 +2843,10 @@
       </c>
       <c r="D99" s="8"/>
       <c r="E99" s="3"/>
-      <c r="F99" s="23"/>
+      <c r="F99" s="22"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="37">
+      <c r="A100" s="36">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
@@ -2723,10 +2858,10 @@
       </c>
       <c r="D100" s="8"/>
       <c r="E100" s="3"/>
-      <c r="F100" s="23"/>
+      <c r="F100" s="22"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="37">
+      <c r="A101" s="36">
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
@@ -2738,10 +2873,10 @@
       </c>
       <c r="D101" s="8"/>
       <c r="E101" s="3"/>
-      <c r="F101" s="23"/>
+      <c r="F101" s="22"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="37">
+      <c r="A102" s="36">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
@@ -2753,10 +2888,10 @@
       </c>
       <c r="D102" s="8"/>
       <c r="E102" s="3"/>
-      <c r="F102" s="23"/>
+      <c r="F102" s="22"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="37">
+      <c r="A103" s="36">
         <f t="shared" si="2"/>
         <v>71</v>
       </c>
@@ -2768,10 +2903,10 @@
       </c>
       <c r="D103" s="8"/>
       <c r="E103" s="3"/>
-      <c r="F103" s="23"/>
+      <c r="F103" s="22"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="37">
+      <c r="A104" s="36">
         <f t="shared" si="2"/>
         <v>72</v>
       </c>
@@ -2783,10 +2918,10 @@
       </c>
       <c r="D104" s="8"/>
       <c r="E104" s="3"/>
-      <c r="F104" s="23"/>
+      <c r="F104" s="22"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="37">
+      <c r="A105" s="36">
         <f t="shared" si="2"/>
         <v>73</v>
       </c>
@@ -2798,10 +2933,10 @@
       </c>
       <c r="D105" s="8"/>
       <c r="E105" s="3"/>
-      <c r="F105" s="23"/>
+      <c r="F105" s="22"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="37">
+      <c r="A106" s="36">
         <f t="shared" si="2"/>
         <v>74</v>
       </c>
@@ -2813,10 +2948,10 @@
       </c>
       <c r="D106" s="8"/>
       <c r="E106" s="3"/>
-      <c r="F106" s="23"/>
+      <c r="F106" s="22"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="37">
+      <c r="A107" s="36">
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
@@ -2828,10 +2963,10 @@
       </c>
       <c r="D107" s="8"/>
       <c r="E107" s="3"/>
-      <c r="F107" s="23"/>
+      <c r="F107" s="22"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="37">
+      <c r="A108" s="36">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
@@ -2843,10 +2978,10 @@
       </c>
       <c r="D108" s="8"/>
       <c r="E108" s="3"/>
-      <c r="F108" s="23"/>
+      <c r="F108" s="22"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="37">
+      <c r="A109" s="36">
         <f t="shared" si="2"/>
         <v>77</v>
       </c>
@@ -2858,10 +2993,10 @@
       </c>
       <c r="D109" s="8"/>
       <c r="E109" s="3"/>
-      <c r="F109" s="23"/>
+      <c r="F109" s="22"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="37">
+      <c r="A110" s="36">
         <f t="shared" si="2"/>
         <v>78</v>
       </c>
@@ -2873,10 +3008,10 @@
       </c>
       <c r="D110" s="8"/>
       <c r="E110" s="3"/>
-      <c r="F110" s="23"/>
+      <c r="F110" s="22"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="37">
+      <c r="A111" s="36">
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
@@ -2888,10 +3023,10 @@
       </c>
       <c r="D111" s="8"/>
       <c r="E111" s="3"/>
-      <c r="F111" s="23"/>
+      <c r="F111" s="22"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="37">
+      <c r="A112" s="36">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
@@ -2903,10 +3038,10 @@
       </c>
       <c r="D112" s="8"/>
       <c r="E112" s="3"/>
-      <c r="F112" s="23"/>
+      <c r="F112" s="22"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="37">
+      <c r="A113" s="36">
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
@@ -2918,10 +3053,10 @@
       </c>
       <c r="D113" s="8"/>
       <c r="E113" s="3"/>
-      <c r="F113" s="23"/>
+      <c r="F113" s="22"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="37">
+      <c r="A114" s="36">
         <f t="shared" si="2"/>
         <v>82</v>
       </c>
@@ -2933,40 +3068,40 @@
       </c>
       <c r="D114" s="8"/>
       <c r="E114" s="3"/>
-      <c r="F114" s="23"/>
+      <c r="F114" s="22"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="37">
+      <c r="A115" s="36">
         <f t="shared" si="2"/>
         <v>83</v>
       </c>
       <c r="B115" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C115" s="43" t="s">
+      <c r="C115" s="42" t="s">
         <v>84</v>
       </c>
       <c r="D115" s="8"/>
       <c r="E115" s="3"/>
-      <c r="F115" s="23"/>
+      <c r="F115" s="22"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="37">
+      <c r="A116" s="36">
         <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="B116" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C116" s="38" t="s">
+      <c r="C116" s="37" t="s">
         <v>85</v>
       </c>
       <c r="D116" s="8"/>
       <c r="E116" s="3"/>
-      <c r="F116" s="23"/>
+      <c r="F116" s="22"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="37">
+      <c r="A117" s="36">
         <f t="shared" si="2"/>
         <v>85</v>
       </c>
@@ -2978,10 +3113,10 @@
       </c>
       <c r="D117" s="8"/>
       <c r="E117" s="3"/>
-      <c r="F117" s="23"/>
+      <c r="F117" s="22"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="37">
+      <c r="A118" s="36">
         <f t="shared" si="2"/>
         <v>86</v>
       </c>
@@ -2993,85 +3128,85 @@
       </c>
       <c r="D118" s="8"/>
       <c r="E118" s="3"/>
-      <c r="F118" s="23"/>
+      <c r="F118" s="22"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="37">
+      <c r="A119" s="36">
         <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="B119" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C119" s="38" t="s">
+      <c r="C119" s="37" t="s">
         <v>88</v>
       </c>
       <c r="D119" s="8"/>
       <c r="E119" s="3"/>
-      <c r="F119" s="23"/>
+      <c r="F119" s="22"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="39">
+      <c r="A120" s="38">
         <f t="shared" si="2"/>
         <v>88</v>
       </c>
-      <c r="B120" s="41" t="s">
+      <c r="B120" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="C120" s="41" t="s">
+      <c r="C120" s="40" t="s">
         <v>90</v>
       </c>
       <c r="D120" s="8"/>
       <c r="E120" s="3"/>
-      <c r="F120" s="23"/>
+      <c r="F120" s="22"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="39">
+      <c r="A121" s="38">
         <f t="shared" si="2"/>
         <v>89</v>
       </c>
-      <c r="B121" s="41" t="s">
+      <c r="B121" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="C121" s="41" t="s">
+      <c r="C121" s="40" t="s">
         <v>91</v>
       </c>
       <c r="D121" s="8"/>
       <c r="E121" s="3"/>
-      <c r="F121" s="23"/>
+      <c r="F121" s="22"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="39">
+      <c r="A122" s="38">
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="B122" s="41" t="s">
+      <c r="B122" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="C122" s="41" t="s">
+      <c r="C122" s="40" t="s">
         <v>92</v>
       </c>
       <c r="D122" s="8"/>
       <c r="E122" s="3"/>
-      <c r="F122" s="23"/>
+      <c r="F122" s="22"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="39">
+      <c r="A123" s="38">
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
-      <c r="B123" s="41" t="s">
+      <c r="B123" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="C123" s="41" t="s">
+      <c r="C123" s="40" t="s">
         <v>93</v>
       </c>
       <c r="D123" s="8"/>
       <c r="E123" s="3"/>
-      <c r="F123" s="23"/>
+      <c r="F123" s="22"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="37">
+      <c r="A124" s="36">
         <f t="shared" si="2"/>
         <v>92</v>
       </c>
@@ -3083,10 +3218,10 @@
       </c>
       <c r="D124" s="8"/>
       <c r="E124" s="3"/>
-      <c r="F124" s="23"/>
+      <c r="F124" s="22"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="37">
+      <c r="A125" s="36">
         <f t="shared" si="2"/>
         <v>93</v>
       </c>
@@ -3098,10 +3233,10 @@
       </c>
       <c r="D125" s="8"/>
       <c r="E125" s="3"/>
-      <c r="F125" s="23"/>
+      <c r="F125" s="22"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="37">
+      <c r="A126" s="36">
         <f t="shared" si="2"/>
         <v>94</v>
       </c>
@@ -3113,10 +3248,10 @@
       </c>
       <c r="D126" s="8"/>
       <c r="E126" s="3"/>
-      <c r="F126" s="23"/>
+      <c r="F126" s="22"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="37">
+      <c r="A127" s="36">
         <f t="shared" si="2"/>
         <v>95</v>
       </c>
@@ -3128,10 +3263,10 @@
       </c>
       <c r="D127" s="8"/>
       <c r="E127" s="3"/>
-      <c r="F127" s="23"/>
+      <c r="F127" s="22"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="37">
+      <c r="A128" s="36">
         <f t="shared" si="2"/>
         <v>96</v>
       </c>
@@ -3143,10 +3278,10 @@
       </c>
       <c r="D128" s="8"/>
       <c r="E128" s="3"/>
-      <c r="F128" s="23"/>
+      <c r="F128" s="22"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="37">
+      <c r="A129" s="36">
         <f t="shared" si="2"/>
         <v>97</v>
       </c>
@@ -3158,10 +3293,10 @@
       </c>
       <c r="D129" s="8"/>
       <c r="E129" s="3"/>
-      <c r="F129" s="23"/>
+      <c r="F129" s="22"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="37">
+      <c r="A130" s="36">
         <f t="shared" si="2"/>
         <v>98</v>
       </c>
@@ -3173,10 +3308,10 @@
       </c>
       <c r="D130" s="8"/>
       <c r="E130" s="3"/>
-      <c r="F130" s="23"/>
+      <c r="F130" s="22"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="37">
+      <c r="A131" s="36">
         <f t="shared" si="2"/>
         <v>99</v>
       </c>
@@ -3188,25 +3323,25 @@
       </c>
       <c r="D131" s="8"/>
       <c r="E131" s="3"/>
-      <c r="F131" s="23"/>
+      <c r="F131" s="22"/>
     </row>
     <row r="132" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="39">
+      <c r="A132" s="38">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="B132" s="41" t="s">
+      <c r="B132" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="C132" s="41" t="s">
+      <c r="C132" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D132" s="8"/>
       <c r="E132" s="3"/>
-      <c r="F132" s="23"/>
+      <c r="F132" s="22"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="37">
+      <c r="A133" s="36">
         <f t="shared" si="2"/>
         <v>101</v>
       </c>
@@ -3218,25 +3353,25 @@
       </c>
       <c r="D133" s="8"/>
       <c r="E133" s="3"/>
-      <c r="F133" s="23"/>
+      <c r="F133" s="22"/>
     </row>
     <row r="134" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="37">
+      <c r="A134" s="36">
         <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="B134" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C134" s="44" t="s">
+      <c r="C134" s="10" t="s">
         <v>146</v>
       </c>
       <c r="D134" s="8"/>
       <c r="E134" s="3"/>
-      <c r="F134" s="23"/>
+      <c r="F134" s="22"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="37">
+      <c r="A135" s="36">
         <f t="shared" si="2"/>
         <v>103</v>
       </c>
@@ -3248,10 +3383,10 @@
       </c>
       <c r="D135" s="8"/>
       <c r="E135" s="3"/>
-      <c r="F135" s="23"/>
+      <c r="F135" s="22"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="37">
+      <c r="A136" s="36">
         <f t="shared" si="2"/>
         <v>104</v>
       </c>
@@ -3263,70 +3398,70 @@
       </c>
       <c r="D136" s="8"/>
       <c r="E136" s="3"/>
-      <c r="F136" s="23"/>
+      <c r="F136" s="22"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="39">
+      <c r="A137" s="38">
         <f t="shared" si="2"/>
         <v>105</v>
       </c>
-      <c r="B137" s="41" t="s">
+      <c r="B137" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="C137" s="41" t="s">
+      <c r="C137" s="40" t="s">
         <v>145</v>
       </c>
       <c r="D137" s="8"/>
       <c r="E137" s="3"/>
-      <c r="F137" s="23"/>
+      <c r="F137" s="22"/>
     </row>
     <row r="138" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="39">
+      <c r="A138" s="38">
         <f t="shared" si="2"/>
         <v>106</v>
       </c>
-      <c r="B138" s="41" t="s">
+      <c r="B138" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="C138" s="13" t="s">
+      <c r="C138" s="7" t="s">
         <v>146</v>
       </c>
       <c r="D138" s="8"/>
       <c r="E138" s="3"/>
-      <c r="F138" s="23"/>
+      <c r="F138" s="22"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" s="39">
+      <c r="A139" s="38">
         <f t="shared" si="2"/>
         <v>107</v>
       </c>
-      <c r="B139" s="41" t="s">
+      <c r="B139" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="C139" s="41" t="s">
+      <c r="C139" s="40" t="s">
         <v>115</v>
       </c>
       <c r="D139" s="8"/>
       <c r="E139" s="3"/>
-      <c r="F139" s="23"/>
+      <c r="F139" s="22"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" s="39">
+      <c r="A140" s="38">
         <f t="shared" si="2"/>
         <v>108</v>
       </c>
-      <c r="B140" s="41" t="s">
+      <c r="B140" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="C140" s="41" t="s">
+      <c r="C140" s="40" t="s">
         <v>116</v>
       </c>
       <c r="D140" s="8"/>
       <c r="E140" s="3"/>
-      <c r="F140" s="23"/>
+      <c r="F140" s="22"/>
     </row>
     <row r="141" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="37">
+      <c r="A141" s="36">
         <f t="shared" si="2"/>
         <v>109</v>
       </c>
@@ -3338,74 +3473,74 @@
       </c>
       <c r="D141" s="8"/>
       <c r="E141" s="3"/>
-      <c r="F141" s="23"/>
+      <c r="F141" s="22"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="39">
+      <c r="A142" s="38">
         <f t="shared" ref="A142:A150" si="3">A141+1</f>
         <v>110</v>
       </c>
-      <c r="B142" s="41" t="s">
+      <c r="B142" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="C142" s="41" t="s">
+      <c r="C142" s="40" t="s">
         <v>128</v>
       </c>
       <c r="D142" s="9"/>
       <c r="E142" s="3"/>
-      <c r="F142" s="23"/>
+      <c r="F142" s="22"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="39">
+      <c r="A143" s="38">
         <f t="shared" si="3"/>
         <v>111</v>
       </c>
-      <c r="B143" s="41" t="s">
+      <c r="B143" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="C143" s="41" t="s">
+      <c r="C143" s="40" t="s">
         <v>129</v>
       </c>
       <c r="D143" s="9"/>
       <c r="E143" s="3"/>
-      <c r="F143" s="23"/>
+      <c r="F143" s="22"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" s="39">
+      <c r="A144" s="38">
         <f t="shared" si="3"/>
         <v>112</v>
       </c>
-      <c r="B144" s="41" t="s">
+      <c r="B144" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="C144" s="41" t="s">
+      <c r="C144" s="40" t="s">
         <v>130</v>
       </c>
       <c r="D144" s="9"/>
       <c r="E144" s="3"/>
-      <c r="F144" s="23"/>
+      <c r="F144" s="22"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="39">
+      <c r="A145" s="38">
         <f t="shared" si="3"/>
         <v>113</v>
       </c>
-      <c r="B145" s="41" t="s">
+      <c r="B145" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="C145" s="41" t="s">
+      <c r="C145" s="40" t="s">
         <v>131</v>
       </c>
       <c r="D145" s="9"/>
       <c r="E145" s="3"/>
-      <c r="F145" s="23"/>
+      <c r="F145" s="22"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="37">
+      <c r="A146" s="36">
         <f t="shared" si="3"/>
         <v>114</v>
       </c>
-      <c r="B146" s="45" t="s">
+      <c r="B146" s="43" t="s">
         <v>132</v>
       </c>
       <c r="C146" s="11" t="s">
@@ -3413,44 +3548,44 @@
       </c>
       <c r="D146" s="9"/>
       <c r="E146" s="3"/>
-      <c r="F146" s="23"/>
+      <c r="F146" s="22"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" s="39">
+      <c r="A147" s="38">
         <f t="shared" si="3"/>
         <v>115</v>
       </c>
-      <c r="B147" s="42" t="s">
+      <c r="B147" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="C147" s="41" t="s">
+      <c r="C147" s="40" t="s">
         <v>163</v>
       </c>
       <c r="D147" s="5"/>
       <c r="E147" s="5"/>
-      <c r="F147" s="23"/>
+      <c r="F147" s="22"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" s="39">
+      <c r="A148" s="38">
         <f t="shared" si="3"/>
         <v>116</v>
       </c>
-      <c r="B148" s="42" t="s">
+      <c r="B148" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="C148" s="41" t="s">
+      <c r="C148" s="40" t="s">
         <v>164</v>
       </c>
       <c r="D148" s="5"/>
       <c r="E148" s="5"/>
-      <c r="F148" s="23"/>
+      <c r="F148" s="22"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="37">
+      <c r="A149" s="36">
         <f t="shared" si="3"/>
         <v>117</v>
       </c>
-      <c r="B149" s="46" t="s">
+      <c r="B149" s="44" t="s">
         <v>167</v>
       </c>
       <c r="C149" s="11" t="s">
@@ -3458,26 +3593,2298 @@
       </c>
       <c r="D149" s="5"/>
       <c r="E149" s="5"/>
-      <c r="F149" s="23"/>
+      <c r="F149" s="22"/>
     </row>
     <row r="150" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="47">
+      <c r="A150" s="45">
         <f t="shared" si="3"/>
         <v>118</v>
       </c>
-      <c r="B150" s="48" t="s">
+      <c r="B150" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="C150" s="48" t="s">
+      <c r="C150" s="46" t="s">
         <v>164</v>
       </c>
-      <c r="D150" s="35"/>
-      <c r="E150" s="35"/>
-      <c r="F150" s="36"/>
+      <c r="D150" s="34"/>
+      <c r="E150" s="34"/>
+      <c r="F150" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97149A6F-53D9-4148-83D6-9A1186C178FD}">
+  <dimension ref="A1:F152"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="43.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="87.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="48.140625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="20"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="20"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="20"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="19">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="19">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="22"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="19">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="22"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="21">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="19">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="22"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="20"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="19">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="22"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
+        <v>22</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="20"/>
+    </row>
+    <row r="24" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="19">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="21">
+        <v>24</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="19">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="20"/>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="21">
+        <v>26</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="20"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="23">
+        <v>27</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="27"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="38">
+        <v>1</v>
+      </c>
+      <c r="B33" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="33"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="36">
+        <f>A33+1</f>
+        <v>2</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="22"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="36">
+        <f t="shared" ref="A35:A74" si="0">A34+1</f>
+        <v>3</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="36">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="22"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="22"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="38">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="22"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="22"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="38">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B40" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="22"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="38">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B41" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="22"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="38">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B42" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="22"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="38">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B43" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="22"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="38">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B44" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="22"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="38">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B45" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="22"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="38">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B46" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="38">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B47" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="22"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="36">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="22"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="38">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B49" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="22"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="38">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B50" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="22"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="38">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B51" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="22"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="36">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="54"/>
+      <c r="F52" s="22"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="36">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="54"/>
+      <c r="F53" s="22"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="36">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="54"/>
+      <c r="F54" s="22"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="36">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="54"/>
+      <c r="F55" s="22"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="38">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B56" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="54"/>
+      <c r="F56" s="22"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="38">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B57" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="22"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="38">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B58" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="54"/>
+      <c r="F58" s="22"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="38">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B59" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="D59" s="3"/>
+      <c r="E59" s="54"/>
+      <c r="F59" s="22"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="36">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D60" s="3"/>
+      <c r="E60" s="55"/>
+      <c r="F60" s="60" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="36">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="55"/>
+      <c r="F61" s="61"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="36">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C62" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="61"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="36">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="D63" s="3"/>
+      <c r="E63" s="55"/>
+      <c r="F63" s="61"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="36">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="D64" s="3"/>
+      <c r="E64" s="55"/>
+      <c r="F64" s="61"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="36">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="D65" s="3"/>
+      <c r="E65" s="55"/>
+      <c r="F65" s="61"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="36">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C66" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" s="3"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="61"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="3"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="61"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="36">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C68" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="3"/>
+      <c r="E68" s="55"/>
+      <c r="F68" s="61"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="36">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C69" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="D69" s="3"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="61"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="36">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="D70" s="3"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="61"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="36">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C71" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="D71" s="3"/>
+      <c r="E71" s="55"/>
+      <c r="F71" s="61"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="36">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C72" s="49" t="s">
+        <v>150</v>
+      </c>
+      <c r="D72" s="3"/>
+      <c r="E72" s="55"/>
+      <c r="F72" s="61"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="36">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C73" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="D73" s="3"/>
+      <c r="E73" s="55"/>
+      <c r="F73" s="61"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="36">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C74" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D74" s="3"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="61"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="36">
+        <f>A74+1</f>
+        <v>43</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C75" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="D75" s="3"/>
+      <c r="E75" s="55"/>
+      <c r="F75" s="61"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="36">
+        <f t="shared" ref="A76:A139" si="1">A75+1</f>
+        <v>44</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C76" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="55"/>
+      <c r="F76" s="61"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="36">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C77" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="D77" s="3"/>
+      <c r="E77" s="55"/>
+      <c r="F77" s="61"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="36">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C78" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="D78" s="3"/>
+      <c r="E78" s="55"/>
+      <c r="F78" s="62"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="38">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B79" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C79" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D79" s="3"/>
+      <c r="E79" s="54"/>
+      <c r="F79" s="22"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="38">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B80" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C80" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D80" s="3"/>
+      <c r="E80" s="54"/>
+      <c r="F80" s="22"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="38">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B81" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C81" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="D81" s="3"/>
+      <c r="E81" s="54"/>
+      <c r="F81" s="22"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="36">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C82" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D82" s="3"/>
+      <c r="E82" s="54"/>
+      <c r="F82" s="22"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="36">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C83" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D83" s="3"/>
+      <c r="E83" s="54"/>
+      <c r="F83" s="22"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="36">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C84" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="54"/>
+      <c r="F84" s="22"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="36">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C85" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="D85" s="3"/>
+      <c r="E85" s="54"/>
+      <c r="F85" s="22"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="36">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C86" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D86" s="3"/>
+      <c r="E86" s="54"/>
+      <c r="F86" s="22"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="36">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C87" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="D87" s="3"/>
+      <c r="E87" s="54"/>
+      <c r="F87" s="22"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="36">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="B88" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C88" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="D88" s="3"/>
+      <c r="E88" s="54"/>
+      <c r="F88" s="22"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="36">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C89" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D89" s="3"/>
+      <c r="E89" s="54"/>
+      <c r="F89" s="22"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="36">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C90" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D90" s="3"/>
+      <c r="E90" s="54"/>
+      <c r="F90" s="22"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="36">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C91" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D91" s="3"/>
+      <c r="E91" s="54"/>
+      <c r="F91" s="22"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="36">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C92" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D92" s="3"/>
+      <c r="E92" s="54"/>
+      <c r="F92" s="22"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="36">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="B93" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C93" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D93" s="3"/>
+      <c r="E93" s="54"/>
+      <c r="F93" s="22"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="36">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="B94" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C94" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D94" s="3"/>
+      <c r="E94" s="54"/>
+      <c r="F94" s="22"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="36">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="B95" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C95" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D95" s="3"/>
+      <c r="E95" s="54"/>
+      <c r="F95" s="22"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="36">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C96" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D96" s="3"/>
+      <c r="E96" s="54"/>
+      <c r="F96" s="22"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="36">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="B97" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C97" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="D97" s="3"/>
+      <c r="E97" s="54"/>
+      <c r="F97" s="22"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="36">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C98" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D98" s="3"/>
+      <c r="E98" s="54"/>
+      <c r="F98" s="22"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="36">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="B99" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C99" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="D99" s="3"/>
+      <c r="E99" s="54"/>
+      <c r="F99" s="22"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="36">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="B100" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C100" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D100" s="3"/>
+      <c r="E100" s="54"/>
+      <c r="F100" s="22"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="36">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="B101" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C101" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D101" s="3"/>
+      <c r="E101" s="54"/>
+      <c r="F101" s="22"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="36">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B102" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C102" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="D102" s="3"/>
+      <c r="E102" s="54"/>
+      <c r="F102" s="22"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="36">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="B103" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C103" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D103" s="3"/>
+      <c r="E103" s="54"/>
+      <c r="F103" s="22"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="36">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="B104" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C104" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="D104" s="3"/>
+      <c r="E104" s="54"/>
+      <c r="F104" s="22"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="36">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="B105" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C105" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D105" s="3"/>
+      <c r="E105" s="54"/>
+      <c r="F105" s="22"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="36">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="B106" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C106" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D106" s="3"/>
+      <c r="E106" s="54"/>
+      <c r="F106" s="22"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="36">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C107" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D107" s="3"/>
+      <c r="E107" s="54"/>
+      <c r="F107" s="22"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="36">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="B108" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C108" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="D108" s="3"/>
+      <c r="E108" s="54"/>
+      <c r="F108" s="22"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="36">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C109" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="D109" s="3"/>
+      <c r="E109" s="54"/>
+      <c r="F109" s="22"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="36">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C110" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D110" s="3"/>
+      <c r="E110" s="54"/>
+      <c r="F110" s="22"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="36">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="B111" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C111" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D111" s="3"/>
+      <c r="E111" s="54"/>
+      <c r="F111" s="22"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="36">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="B112" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C112" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D112" s="3"/>
+      <c r="E112" s="54"/>
+      <c r="F112" s="22"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="36">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="B113" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C113" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="D113" s="3"/>
+      <c r="E113" s="54"/>
+      <c r="F113" s="22"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="36">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="B114" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C114" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="D114" s="3"/>
+      <c r="E114" s="54"/>
+      <c r="F114" s="22"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="36">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="B115" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C115" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="D115" s="3"/>
+      <c r="E115" s="54"/>
+      <c r="F115" s="22"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="36">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="B116" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C116" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D116" s="3"/>
+      <c r="E116" s="54"/>
+      <c r="F116" s="22"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="36">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="B117" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C117" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="D117" s="3"/>
+      <c r="E117" s="54"/>
+      <c r="F117" s="22"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="36">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="B118" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C118" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="D118" s="3"/>
+      <c r="E118" s="54"/>
+      <c r="F118" s="22"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="36">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="B119" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C119" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="D119" s="3"/>
+      <c r="E119" s="54"/>
+      <c r="F119" s="22"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="38">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="B120" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C120" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="D120" s="3"/>
+      <c r="E120" s="54"/>
+      <c r="F120" s="22"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="38">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="B121" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C121" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D121" s="3"/>
+      <c r="E121" s="54"/>
+      <c r="F121" s="22"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="38">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B122" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C122" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="D122" s="3"/>
+      <c r="E122" s="54"/>
+      <c r="F122" s="22"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="38">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="B123" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C123" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="D123" s="3"/>
+      <c r="E123" s="54"/>
+      <c r="F123" s="22"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="36">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="B124" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C124" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="D124" s="3"/>
+      <c r="E124" s="54"/>
+      <c r="F124" s="22"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="36">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B125" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C125" s="49" t="s">
+        <v>138</v>
+      </c>
+      <c r="D125" s="3"/>
+      <c r="E125" s="54"/>
+      <c r="F125" s="22"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="36">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B126" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C126" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="D126" s="3"/>
+      <c r="E126" s="54"/>
+      <c r="F126" s="22"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="36">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C127" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="D127" s="3"/>
+      <c r="E127" s="54"/>
+      <c r="F127" s="22"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="36">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C128" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="D128" s="3"/>
+      <c r="E128" s="54"/>
+      <c r="F128" s="22"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="36">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="B129" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C129" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="D129" s="3"/>
+      <c r="E129" s="54"/>
+      <c r="F129" s="22"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="36">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="B130" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C130" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="D130" s="3"/>
+      <c r="E130" s="54"/>
+      <c r="F130" s="22"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="36">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="B131" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C131" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="D131" s="3"/>
+      <c r="E131" s="54"/>
+      <c r="F131" s="22"/>
+    </row>
+    <row r="132" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="38">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="B132" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="C132" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="D132" s="3"/>
+      <c r="E132" s="54"/>
+      <c r="F132" s="22"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="36">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="B133" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C133" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="D133" s="3"/>
+      <c r="E133" s="54"/>
+      <c r="F133" s="22"/>
+    </row>
+    <row r="134" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="36">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="B134" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C134" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="D134" s="3"/>
+      <c r="E134" s="54"/>
+      <c r="F134" s="22"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="36">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="B135" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C135" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="D135" s="3"/>
+      <c r="E135" s="54"/>
+      <c r="F135" s="22"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="36">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="B136" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C136" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="D136" s="3"/>
+      <c r="E136" s="54"/>
+      <c r="F136" s="22"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="38">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="B137" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="C137" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="D137" s="3"/>
+      <c r="E137" s="54"/>
+      <c r="F137" s="22"/>
+    </row>
+    <row r="138" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="38">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="B138" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="C138" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="D138" s="3"/>
+      <c r="E138" s="54"/>
+      <c r="F138" s="22"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="38">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="B139" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="C139" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="D139" s="3"/>
+      <c r="E139" s="54"/>
+      <c r="F139" s="22"/>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="38">
+        <f t="shared" ref="A140:A150" si="2">A139+1</f>
+        <v>108</v>
+      </c>
+      <c r="B140" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="C140" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="D140" s="3"/>
+      <c r="E140" s="54"/>
+      <c r="F140" s="22"/>
+    </row>
+    <row r="141" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="36">
+        <f t="shared" si="2"/>
+        <v>109</v>
+      </c>
+      <c r="B141" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C141" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="D141" s="3"/>
+      <c r="E141" s="54"/>
+      <c r="F141" s="22"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="38">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="B142" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C142" s="50" t="s">
+        <v>128</v>
+      </c>
+      <c r="D142" s="5"/>
+      <c r="E142" s="54"/>
+      <c r="F142" s="22"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="38">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+      <c r="B143" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C143" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="D143" s="5"/>
+      <c r="E143" s="54"/>
+      <c r="F143" s="22"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="38">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+      <c r="B144" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C144" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="D144" s="5"/>
+      <c r="E144" s="54"/>
+      <c r="F144" s="22"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" s="38">
+        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+      <c r="B145" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C145" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="D145" s="5"/>
+      <c r="E145" s="54"/>
+      <c r="F145" s="22"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="36">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="B146" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C146" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="D146" s="5"/>
+      <c r="E146" s="54"/>
+      <c r="F146" s="22"/>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="38">
+        <f t="shared" si="2"/>
+        <v>115</v>
+      </c>
+      <c r="B147" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="C147" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="D147" s="5"/>
+      <c r="E147" s="56"/>
+      <c r="F147" s="22"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="38">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+      <c r="B148" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="C148" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="D148" s="5"/>
+      <c r="E148" s="56"/>
+      <c r="F148" s="22"/>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="36">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+      <c r="B149" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="C149" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="D149" s="5"/>
+      <c r="E149" s="56"/>
+      <c r="F149" s="22"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="36">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+      <c r="B150" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C150" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D150" s="5"/>
+      <c r="E150" s="5"/>
+      <c r="F150" s="22"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="58">
+        <v>119</v>
+      </c>
+      <c r="B151" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="C151" s="57" t="s">
+        <v>169</v>
+      </c>
+      <c r="D151" s="5"/>
+      <c r="E151" s="5"/>
+      <c r="F151" s="22"/>
+    </row>
+    <row r="152" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="59">
+        <v>120</v>
+      </c>
+      <c r="B152" s="46" t="s">
+        <v>170</v>
+      </c>
+      <c r="C152" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="D152" s="34"/>
+      <c r="E152" s="34"/>
+      <c r="F152" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F60:F78"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3730,15 +6137,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="58c86f0d-105b-411a-9dc4-426c473fb672">
@@ -3749,14 +6147,50 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB7AD9D2-8421-4F0A-93A1-9A5CAA109487}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB7AD9D2-8421-4F0A-93A1-9A5CAA109487}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="58c86f0d-105b-411a-9dc4-426c473fb672"/>
+    <ds:schemaRef ds:uri="3a859602-8111-4d99-a327-232507121e0e"/>
+    <ds:schemaRef ds:uri="a7bc6c04-a6f3-4b85-abcc-278c78dc556b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B1F353B-8BDB-4EB0-837B-7EBD0A36570B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{734F3C5A-1958-4943-BD21-9C279E7DA924}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="58c86f0d-105b-411a-9dc4-426c473fb672"/>
+    <ds:schemaRef ds:uri="a7bc6c04-a6f3-4b85-abcc-278c78dc556b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{734F3C5A-1958-4943-BD21-9C279E7DA924}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B1F353B-8BDB-4EB0-837B-7EBD0A36570B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Added requirement for Data Echo and Data Received Echo to be sent at least 3 times and received at least once correctly Implementation compliant with 1.1 LTPI Specification. Updated User Guide. Signed-off-by: Katarzyna Krzewska <katarzyna.krzewska@intel.com>
</commit_message>
<xml_diff>
--- a/docs/LTPI_test_plan.xlsx
+++ b/docs/LTPI_test_plan.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/katarzyna_krzewska_intel_com/Documents/Documents/LTPI/LTPI_dokumentacja/LTPI_src_OCP_release/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="615" documentId="8_{1719A915-AC1B-49BB-AA9D-1482FFA7DE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A543862-F5AF-4F6F-8638-5DC670249272}"/>
+  <xr:revisionPtr revIDLastSave="616" documentId="8_{1719A915-AC1B-49BB-AA9D-1482FFA7DE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{808484B4-BCEE-4699-A104-6AEB124273AD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{B27309D5-33D0-42FB-BA45-6062C8749EE3}"/>
+    <workbookView xWindow="3390" yWindow="5670" windowWidth="20730" windowHeight="11835" activeTab="1" xr2:uid="{B27309D5-33D0-42FB-BA45-6062C8749EE3}"/>
   </bookViews>
   <sheets>
     <sheet name="LTPI 1.0" sheetId="1" r:id="rId1"/>
-    <sheet name="LTPI 1.09" sheetId="2" r:id="rId2"/>
+    <sheet name="LTPI 1.09 &amp; 1.1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1032,15 +1032,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1062,6 +1053,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -3636,22 +3636,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="68" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4062,22 +4062,22 @@
       <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="64" t="s">
+      <c r="A32" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="65" t="s">
+      <c r="B32" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="65" t="s">
+      <c r="C32" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="63" t="s">
+      <c r="D32" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="66" t="s">
+      <c r="E32" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="67" t="s">
+      <c r="F32" s="64" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4498,7 +4498,7 @@
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="55"/>
-      <c r="F60" s="60" t="s">
+      <c r="F60" s="69" t="s">
         <v>171</v>
       </c>
     </row>
@@ -4515,7 +4515,7 @@
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="55"/>
-      <c r="F61" s="61"/>
+      <c r="F61" s="70"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="36">
@@ -4530,7 +4530,7 @@
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="55"/>
-      <c r="F62" s="61"/>
+      <c r="F62" s="70"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="36">
@@ -4545,7 +4545,7 @@
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="55"/>
-      <c r="F63" s="61"/>
+      <c r="F63" s="70"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="36">
@@ -4560,7 +4560,7 @@
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="55"/>
-      <c r="F64" s="61"/>
+      <c r="F64" s="70"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="36">
@@ -4575,7 +4575,7 @@
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="55"/>
-      <c r="F65" s="61"/>
+      <c r="F65" s="70"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="36">
@@ -4590,7 +4590,7 @@
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="55"/>
-      <c r="F66" s="61"/>
+      <c r="F66" s="70"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="36">
@@ -4605,7 +4605,7 @@
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="55"/>
-      <c r="F67" s="61"/>
+      <c r="F67" s="70"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="36">
@@ -4620,7 +4620,7 @@
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="55"/>
-      <c r="F68" s="61"/>
+      <c r="F68" s="70"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="36">
@@ -4635,7 +4635,7 @@
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="55"/>
-      <c r="F69" s="61"/>
+      <c r="F69" s="70"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="36">
@@ -4650,7 +4650,7 @@
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="55"/>
-      <c r="F70" s="61"/>
+      <c r="F70" s="70"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="36">
@@ -4665,7 +4665,7 @@
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="55"/>
-      <c r="F71" s="61"/>
+      <c r="F71" s="70"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="36">
@@ -4680,7 +4680,7 @@
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="55"/>
-      <c r="F72" s="61"/>
+      <c r="F72" s="70"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="36">
@@ -4695,7 +4695,7 @@
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="55"/>
-      <c r="F73" s="61"/>
+      <c r="F73" s="70"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="36">
@@ -4710,7 +4710,7 @@
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="55"/>
-      <c r="F74" s="61"/>
+      <c r="F74" s="70"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="36">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="55"/>
-      <c r="F75" s="61"/>
+      <c r="F75" s="70"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="36">
@@ -4740,7 +4740,7 @@
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="55"/>
-      <c r="F76" s="61"/>
+      <c r="F76" s="70"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="36">
@@ -4755,7 +4755,7 @@
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="55"/>
-      <c r="F77" s="61"/>
+      <c r="F77" s="70"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="36">
@@ -4770,7 +4770,7 @@
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="55"/>
-      <c r="F78" s="62"/>
+      <c r="F78" s="71"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="38">
@@ -6137,6 +6137,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="58c86f0d-105b-411a-9dc4-426c473fb672">
@@ -6145,15 +6154,6 @@
     <TaxCatchAll xmlns="a7bc6c04-a6f3-4b85-abcc-278c78dc556b" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6177,6 +6177,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B1F353B-8BDB-4EB0-837B-7EBD0A36570B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{734F3C5A-1958-4943-BD21-9C279E7DA924}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -6185,12 +6193,4 @@
     <ds:schemaRef ds:uri="a7bc6c04-a6f3-4b85-abcc-278c78dc556b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B1F353B-8BDB-4EB0-837B-7EBD0A36570B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>